<commit_message>
added proc board connector to BOM
</commit_message>
<xml_diff>
--- a/E17-06-PDU/PDU Digikey BOM.xlsx
+++ b/E17-06-PDU/PDU Digikey BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Quantity</t>
   </si>
@@ -301,6 +301,15 @@
   </si>
   <si>
     <t>P56ACT-ND</t>
+  </si>
+  <si>
+    <t>A115899CT-ND</t>
+  </si>
+  <si>
+    <t>PROC BOARD CONNECTOR</t>
+  </si>
+  <si>
+    <t>CONN FEMALE 67POS 0.020 GOLD</t>
   </si>
 </sst>
 </file>
@@ -1141,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1589,6 +1598,20 @@
         <v>85</v>
       </c>
     </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>